<commit_message>
20201203　朱　KFC　5
</commit_message>
<xml_diff>
--- a/精算.xlsx
+++ b/精算.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="307">
   <si>
     <t>その他</t>
     <rPh sb="2" eb="3">
@@ -2286,6 +2286,10 @@
     <t>KFC</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>KFC</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -2870,7 +2874,7 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D250" sqref="D250"/>
+      <selection activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -2921,7 +2925,7 @@
       </c>
       <c r="F2" s="16">
         <f t="shared" ref="F2:G2" si="1">SUM(F3:F930)</f>
-        <v>226.3</v>
+        <v>231.3</v>
       </c>
       <c r="G2" s="16">
         <f t="shared" si="1"/>
@@ -5317,7 +5321,7 @@
       </c>
       <c r="F257" s="3">
         <f>'202012'!$O$2</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G257" s="3">
         <f>'202012'!$R$2</f>
@@ -14245,7 +14249,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -14329,7 +14333,7 @@
       <c r="M2" s="43"/>
       <c r="O2" s="42">
         <f>SUM(P:P)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P2" s="43"/>
       <c r="R2" s="42">
@@ -14395,8 +14399,12 @@
       <c r="J5" s="8"/>
       <c r="L5" s="17"/>
       <c r="M5" s="8"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="P5" s="8">
+        <v>5</v>
+      </c>
       <c r="R5" s="17"/>
       <c r="S5" s="8"/>
     </row>
@@ -14998,11 +15006,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="O2:P2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:G1"/>
@@ -15010,6 +15013,11 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="R1:S1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>